<commit_message>
recap result of ELMo -BiLSTM
</commit_message>
<xml_diff>
--- a/output-2/drone-polysemi/bilstm/evaluation_bilstm.xlsx
+++ b/output-2/drone-polysemi/bilstm/evaluation_bilstm.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,107 +593,107 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.104089</t>
+          <t>0.897554</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.130536</t>
+          <t>0.888048</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.086553</t>
+          <t>0.907264</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.210923</t>
+          <t>0.980583</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.130536</t>
+          <t>0.971154</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.54902</t>
+          <t>0.990196</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.653333</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.620253</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.690141</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.864865</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.987654</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.769231</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.981366</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.975309</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.868687</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.781818</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.977273</t>
         </is>
       </c>
     </row>
@@ -1756,12 +1756,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>lstm</t>
+          <t>cnn</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>bert</t>
+          <t>elmo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1776,107 +1776,107 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.883137</t>
+          <t>0.878549</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.896497</t>
+          <t>0.89694</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.87017</t>
+          <t>0.860896</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.964824</t>
+          <t>0.964467</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.989691</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.941176</t>
+          <t>0.931373</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0.652778</t>
+          <t>0.552239</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.643836</t>
+          <t>0.587302</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0.661972</t>
+          <t>0.521127</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>0.746988</t>
+          <t>0.758621</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
+          <t>0.942857</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0.634615</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>0.939597</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0.985915</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>0.897436</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.993711</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>0.596154</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>0.938776</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>0.884615</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>0.9875</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>0.9875</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>0.9875</t>
-        </is>
-      </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>0.876254</t>
+          <t>0.885135</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>0.784431</t>
+          <t>0.79878</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
@@ -1888,12 +1888,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>adatrans</t>
+          <t>lstm</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>glove</t>
+          <t>bert</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1908,77 +1908,77 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.869906</t>
+          <t>0.883137</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.882353</t>
+          <t>0.896497</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.857805</t>
+          <t>0.87017</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.954774</t>
+          <t>0.964824</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0.979381</t>
+          <t>0.989691</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0.931373</t>
+          <t>0.941176</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0.492308</t>
+          <t>0.652778</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.542373</t>
+          <t>0.643836</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0.450704</t>
+          <t>0.661972</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>0.822222</t>
+          <t>0.746988</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0.973684</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>0.711538</t>
+          <t>0.596154</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>0.92</t>
+          <t>0.938776</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>0.958333</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -1988,44 +1988,44 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>0.971963</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>0.968944</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>0.975</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>0.871622</t>
+          <t>0.876254</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>0.786585</t>
+          <t>0.784431</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>0.977273</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>lstm</t>
+          <t>adatrans</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>elmo</t>
+          <t>glove</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2040,112 +2040,112 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.096654</t>
+          <t>0.869906</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.121212</t>
+          <t>0.882353</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.080371</t>
+          <t>0.857805</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.195857</t>
+          <t>0.954774</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0.121212</t>
+          <t>0.979381</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0.509804</t>
+          <t>0.931373</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.492308</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.542373</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.450704</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.822222</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.973684</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.711538</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.92</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.958333</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.971963</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.968944</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.871622</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.786585</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.977273</t>
         </is>
       </c>
     </row>
@@ -2172,112 +2172,112 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.104876</t>
+          <t>0.890432</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.129545</t>
+          <t>0.88906</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.088099</t>
+          <t>0.891808</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.980198</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.970588</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.552239</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.587302</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.521127</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>0.266667</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
+          <t>0.954545</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>0.807692</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0.924138</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>0.153846</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.858974</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>0.196172</t>
+          <t>0.981481</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>0.158915</t>
+          <t>0.969512</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>0.25625</t>
+          <t>0.99375</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.876254</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.784431</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>glove</t>
+          <t>elmo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2304,57 +2304,57 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.843922</t>
+          <t>0.892664</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.856688</t>
+          <t>0.891975</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.83153</t>
+          <t>0.893354</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.975369</t>
+          <t>0.951456</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.980198</t>
+          <t>0.942308</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0.970588</t>
+          <t>0.960784</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0.496124</t>
+          <t>0.604317</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.551724</t>
+          <t>0.617647</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>0.450704</t>
+          <t>0.591549</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>0.761905</t>
+          <t>0.850829</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -2364,52 +2364,52 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>0.615385</t>
+          <t>0.740385</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>0.92</t>
+          <t>0.934211</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>0.958333</t>
+          <t>0.959459</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>0.884615</t>
+          <t>0.910256</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>0.897196</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>0.89441</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>0.855263</t>
+          <t>0.888889</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>0.755814</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>0.984848</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>bert</t>
+          <t>glove</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2441,52 +2441,52 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0.88701</t>
+          <t>0.843922</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.882263</t>
+          <t>0.856688</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.891808</t>
+          <t>0.83153</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.97</t>
+          <t>0.975369</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.989796</t>
+          <t>0.980198</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0.95098</t>
+          <t>0.970588</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0.57554</t>
+          <t>0.496124</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0.588235</t>
+          <t>0.551724</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>0.56338</t>
+          <t>0.450704</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>0.893617</t>
+          <t>0.761905</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -2496,17 +2496,17 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>0.807692</t>
+          <t>0.615385</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>0.901961</t>
+          <t>0.92</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>0.92</t>
+          <t>0.958333</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
@@ -2516,44 +2516,44 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>0.96</t>
+          <t>0.897196</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>0.945455</t>
+          <t>0.89441</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>0.975</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>0.885135</t>
+          <t>0.855263</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>0.79878</t>
+          <t>0.755814</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>0.992424</t>
+          <t>0.984848</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>cnn</t>
+          <t>lstm</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>elmo</t>
+          <t>bert</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2573,107 +2573,107 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0.214208</t>
+          <t>0.88701</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.365672</t>
+          <t>0.882263</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.151468</t>
+          <t>0.891808</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.97</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.989796</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.95098</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.57554</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.588235</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.56338</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.893617</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.807692</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.901961</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.92</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>0.521505</t>
+          <t>0.96</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>0.457547</t>
+          <t>0.945455</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>0.60625</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>0.010989</t>
+          <t>0.885135</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.79878</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>0.007576</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -2700,119 +2700,119 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0.095949</t>
+          <t>0.899848</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.154639</t>
+          <t>0.883756</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.069552</t>
+          <t>0.916538</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.969697</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.941176</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.671233</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.653333</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.690141</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.940594</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.969388</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.913462</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.90411</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.970588</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.846154</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>0.210773</t>
+          <t>0.972308</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>0.168539</t>
+          <t>0.957576</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>0.28125</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.86755</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.770588</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>adatrans</t>
+          <t>cnn</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2832,124 +2832,124 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0.088154</t>
+          <t>0.887865</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.108597</t>
+          <t>0.882443</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.074189</t>
+          <t>0.893354</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.990099</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.980392</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.518519</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.546875</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.492958</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.873096</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.924731</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.826923</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>0.162988</t>
+          <t>0.978056</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>0.111888</t>
+          <t>0.981132</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.870432</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.775148</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>lstm</t>
+          <t>adatrans</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>glove</t>
+          <t>elmo</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2964,47 +2964,47 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0.843922</t>
+          <t>0.882398</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.856688</t>
+          <t>0.877676</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.83153</t>
+          <t>0.887172</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.951456</t>
+          <t>0.980583</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0.942308</t>
+          <t>0.971154</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>0.960784</t>
+          <t>0.990196</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>0.526316</t>
+          <t>0.503597</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0.564516</t>
+          <t>0.514706</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -3014,74 +3014,74 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>0.745562</t>
+          <t>0.844444</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>0.969231</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>0.605769</t>
+          <t>0.730769</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>0.918919</t>
+          <t>0.947368</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>0.971429</t>
+          <t>0.972973</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>0.871795</t>
+          <t>0.923077</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>0.90566</t>
+          <t>0.975309</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>0.911392</t>
+          <t>0.963415</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>0.863787</t>
+          <t>0.88</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>0.769231</t>
+          <t>0.785714</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>0.984848</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>adatrans</t>
+          <t>lstm</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>elmo</t>
+          <t>glove</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -3096,124 +3096,124 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0.124555</t>
+          <t>0.843922</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.146751</t>
+          <t>0.856688</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.108192</t>
+          <t>0.83153</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.951456</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.942308</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.960784</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.526316</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.564516</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.492958</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.745562</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.969231</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.605769</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>0.141304</t>
+          <t>0.918919</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>0.089655</t>
+          <t>0.971429</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>0.333333</t>
+          <t>0.871795</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>0.345098</t>
+          <t>0.90566</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>0.463158</t>
+          <t>0.911392</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>0.275</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.863787</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.769231</t>
         </is>
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.984848</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>cnn</t>
+          <t>adatrans</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>bert</t>
+          <t>elmo</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -3228,32 +3228,32 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0.89977</t>
+          <t>0.898705</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.890909</t>
+          <t>0.885886</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0.90881</t>
+          <t>0.911901</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.980198</t>
+          <t>0.985075</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.99</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -3263,27 +3263,27 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>0.652778</t>
+          <t>0.671233</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.643836</t>
+          <t>0.653333</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>0.661972</t>
+          <t>0.690141</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>0.884211</t>
+          <t>0.888889</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>0.976744</t>
+          <t>0.988235</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -3293,42 +3293,42 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>0.953642</t>
+          <t>0.938776</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>0.986301</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>0.923077</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>0.987578</t>
+          <t>0.957576</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>0.981481</t>
+          <t>0.929412</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>0.99375</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>0.86755</t>
+          <t>0.873333</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>0.770588</t>
+          <t>0.779762</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
@@ -3360,37 +3360,37 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.875776</t>
+          <t>0.89977</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.879875</t>
+          <t>0.890909</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0.871716</t>
+          <t>0.90881</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.953271</t>
+          <t>0.980198</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0.910714</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.970588</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -3410,62 +3410,62 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>0.77193</t>
+          <t>0.884211</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>0.985075</t>
+          <t>0.976744</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>0.634615</t>
+          <t>0.807692</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>0.873239</t>
+          <t>0.953642</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>0.96875</t>
+          <t>0.986301</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>0.794872</t>
+          <t>0.923077</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>0.9875</t>
+          <t>0.987578</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>0.9875</t>
+          <t>0.981481</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>0.9875</t>
+          <t>0.99375</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>0.868687</t>
+          <t>0.86755</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>0.781818</t>
+          <t>0.770588</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>0.977273</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>elmo</t>
+          <t>bert</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3492,124 +3492,124 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0.089219</t>
+          <t>0.875776</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.111888</t>
+          <t>0.879875</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0.074189</t>
+          <t>0.871716</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.953271</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.910714</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.652778</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.643836</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.661972</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.77193</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.985075</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.634615</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.873239</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.96875</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.794872</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>0.162988</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>0.111888</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.868687</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.781818</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.977273</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>adatrans</t>
+          <t>cnn</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>bert</t>
+          <t>elmo</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3624,77 +3624,77 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.892142</t>
+          <t>0.897321</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0.889401</t>
+          <t>0.865136</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.8949</t>
+          <t>0.931994</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.96</t>
+          <t>0.966507</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0.979592</t>
+          <t>0.943925</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>0.941176</t>
+          <t>0.990196</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>0.652778</t>
+          <t>0.719577</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.643836</t>
+          <t>0.576271</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>0.661972</t>
+          <t>0.957746</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>0.84153</t>
+          <t>0.858696</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>0.974684</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>0.740385</t>
+          <t>0.759615</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>0.933333</t>
+          <t>0.939597</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>0.972222</t>
+          <t>0.985915</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
@@ -3704,39 +3704,39 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>0.9875</t>
+          <t>0.987342</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>0.9875</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>0.9875</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>0.870432</t>
+          <t>0.868687</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>0.775148</t>
+          <t>0.781818</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>0.992424</t>
+          <t>0.977273</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>cnn</t>
+          <t>adatrans</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3756,47 +3756,47 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0.866106</t>
+          <t>0.892142</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0.857576</t>
+          <t>0.889401</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0.874807</t>
+          <t>0.8949</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.932692</t>
+          <t>0.96</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0.915094</t>
+          <t>0.979592</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>0.95098</t>
+          <t>0.941176</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>0.591195</t>
+          <t>0.652778</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.534091</t>
+          <t>0.643836</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -3806,74 +3806,74 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>0.81768</t>
+          <t>0.84153</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>0.961039</t>
+          <t>0.974684</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>0.711538</t>
+          <t>0.740385</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>0.911565</t>
+          <t>0.933333</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>0.971014</t>
+          <t>0.972222</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>0.858974</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>0.931148</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>0.97931</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>0.8875</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>0.872483</t>
+          <t>0.870432</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>0.783133</t>
+          <t>0.775148</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>0.984848</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>lstm</t>
+          <t>cnn</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>glove</t>
+          <t>bert</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -3893,107 +3893,107 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0.865672</t>
+          <t>0.866106</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0.880192</t>
+          <t>0.857576</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0.851623</t>
+          <t>0.874807</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.970588</t>
+          <t>0.932692</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0.970588</t>
+          <t>0.915094</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>0.970588</t>
+          <t>0.95098</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>0.530303</t>
+          <t>0.591195</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.57377</t>
+          <t>0.534091</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>0.492958</t>
+          <t>0.661972</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>0.723926</t>
+          <t>0.81768</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.961039</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>0.567308</t>
+          <t>0.711538</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>0.95302</t>
+          <t>0.911565</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.971014</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>0.910256</t>
+          <t>0.858974</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>0.981132</t>
+          <t>0.931148</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>0.987342</t>
+          <t>0.97931</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>0.975</t>
+          <t>0.8875</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>0.85342</t>
+          <t>0.872483</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>0.748571</t>
+          <t>0.783133</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>0.992424</t>
+          <t>0.984848</t>
         </is>
       </c>
     </row>
@@ -4005,127 +4005,259 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>glove</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>unscaled</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>bilstm</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>0.865672</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0.880192</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0.851623</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0.970588</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.970588</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>0.970588</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0.530303</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>0.57377</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>0.492958</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>0.723926</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>0.567308</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>0.95302</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>0.910256</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>0.981132</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>0.987342</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>0.975</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>0.85342</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>0.748571</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>0.992424</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>lstm</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>elmo</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>unscaled</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>bilstm</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>0.145009</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>0.185542</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>0.119011</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>0.26383</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>0.233083</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>0.303922</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>0.148148</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>0.142857</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>0.153846</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>0.184615</t>
-        </is>
-      </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>0.181818</t>
-        </is>
-      </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>0.1875</t>
-        </is>
-      </c>
-      <c r="X28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="Z28" t="inlineStr">
-        <is>
-          <t>0.0</t>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>0.896024</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.886536</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0.905719</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0.97</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>0.989796</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0.95098</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0.652778</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0.643836</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>0.661972</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>0.879581</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>0.965517</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>0.807692</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>0.923077</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>0.968944</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>0.962963</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>0.975</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>0.863787</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>0.769231</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>0.984848</t>
         </is>
       </c>
     </row>

</xml_diff>